<commit_message>
Scripting DPLKKEU011-001 and DPLKKEU012-001
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKKEU009-001 - Keuangan - Approval Pembayaran Investasi.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKKEU009-001 - Keuangan - Approval Pembayaran Investasi.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2869AB18-0B0B-4CF7-9E57-EA8501D3C1D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81658E90-5E0C-4ED5-85EB-EFEA6F04B141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DPLKKEU009" sheetId="2" r:id="rId1"/>
+    <sheet name="DPLKKEU009-001" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -76,48 +76,48 @@
     <t>DPLKKEU009-001</t>
   </si>
   <si>
-    <t>Approval Settlement Transaksi Penempatan Deposito BANK BNI - JPU Jakarta Pusat DLK/3/3251 PRI01-Deposito Pasar Uang DOC -- Keuangan Investasi - Proses - Approval Pembayaran Investasi</t>
-  </si>
-  <si>
     <t>Data sesuai dan proses approval berhasil</t>
+  </si>
+  <si>
+    <t>Keuangan Investasi</t>
+  </si>
+  <si>
+    <t>Approval Pembayaran Investasi</t>
+  </si>
+  <si>
+    <t>KODE_PEMBAYARAN</t>
+  </si>
+  <si>
+    <t>Normal - Approval Pembayaran Investasi</t>
+  </si>
+  <si>
+    <t>KETERANGAN</t>
+  </si>
+  <si>
+    <t>Approval Settlement Transaksi Penempatan Deposito BANK BNI - JPU Jakarta Pusat DLK/3/3162 PRI01-Deposito Pasar Uang DOC -- Keuangan Investasi - Proses - Approval Pembayaran Investasi</t>
   </si>
   <si>
     <t>Username : 31816;
 Password : bni1234;
 Role : 09;
-Search : INV.DEP.PEN.010;
-Kode Pembayaran : BC001-O-22-08-00160;
+Search : INV.DEP.PEN.012;
+Kode Pembayaran : BC001-O-22-08-00012;
 Entitas : DPLKBNI : DPLK PT. BNI (Persero) Tbk.;
-Kantor ID : 750 : DLK;
+Kantor ID : 216 : PASURUAN;
 Kode Buku : BC001;
 Nama Bank : Bank Negara Indonesia 1946;
 No Rekening : 1000564390;
 Produk/Cluster : Deposito Pasar Uang;
 Mata Uang : IDR : Rupiah;
-Tanggal RK : 04/08/2022;
-Nominal Pembayaran : 30.000.000,00;
-Keterangan : INV.DEP.PEN.010 EDIT DATA DPLK PT. BNI (Persero) Tbk. Deposito Pasar Uang</t>
-  </si>
-  <si>
-    <t>Keuangan Investasi</t>
-  </si>
-  <si>
-    <t>Approval Pembayaran Investasi</t>
-  </si>
-  <si>
-    <t>KODE_PEMBAYARAN</t>
-  </si>
-  <si>
-    <t>BC001-O-22-08-00160</t>
-  </si>
-  <si>
-    <t>Normal - Approval Pembayaran Investasi</t>
-  </si>
-  <si>
-    <t>KETERANGAN</t>
-  </si>
-  <si>
-    <t>INV.DEP.PEN.010</t>
+Tanggal RK : 05/08/2022;
+Nominal Pembayaran : 40.000.000.000,00;
+Keterangan : INV.DEP.PEN.012 DPLK PT. BNI (Persero) Tbk. Deposito Pasar Uang</t>
+  </si>
+  <si>
+    <t>BC001-O-22-08-00012</t>
+  </si>
+  <si>
+    <t>INV.DEP.PEN.012</t>
   </si>
 </sst>
 </file>
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +536,7 @@
     <col min="10" max="10" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -593,10 +593,10 @@
         <v>13</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="330" x14ac:dyDescent="0.25">
@@ -607,16 +607,16 @@
         <v>17</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="G2" s="4">
         <v>31816</v>
@@ -634,13 +634,13 @@
         <v>12</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="O2" s="10" t="s">
         <v>27</v>
@@ -665,7 +665,6 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="K3" s="5"/>
-      <c r="M3" s="4"/>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="9"/>

</xml_diff>